<commit_message>
BasePower schematic mostly done
</commit_message>
<xml_diff>
--- a/design_simulations/TPS552892/TPS552892-CALCULATION-TOOL-V1.0.xlsx
+++ b/design_simulations/TPS552892/TPS552892-CALCULATION-TOOL-V1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Alex\Documents\Electronics Projects\Modular Audio\design_simulations\TPS552892\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96047C16-277D-4DCF-BDDF-64B579D90496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A02C45E-DD04-4293-805A-CD98EB43E7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,9 +211,6 @@
     <t>Minimum output capacitance needed for Vout ripple requirement</t>
   </si>
   <si>
-    <t>Internal</t>
-  </si>
-  <si>
     <t>Efficiency estimate. Correct it after getting the calculated efficiency</t>
   </si>
   <si>
@@ -954,6 +951,9 @@
   </si>
   <si>
     <t>The inductor average current at minmum Vin.</t>
+  </si>
+  <si>
+    <t>External</t>
   </si>
 </sst>
 </file>
@@ -3505,8 +3505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S69" sqref="S69"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -3551,7 +3551,7 @@
     <row r="2" spans="1:17" ht="16.5" thickTop="1">
       <c r="A2" s="48"/>
       <c r="B2" s="145" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C2" s="146"/>
       <c r="D2" s="146"/>
@@ -3572,7 +3572,7 @@
     <row r="3" spans="1:17">
       <c r="A3" s="48"/>
       <c r="B3" s="148" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C3" s="149"/>
       <c r="D3" s="149"/>
@@ -3631,7 +3631,7 @@
     <row r="6" spans="1:17" ht="13.15" customHeight="1">
       <c r="A6" s="48"/>
       <c r="B6" s="151" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C6" s="152"/>
       <c r="D6" s="152"/>
@@ -3673,7 +3673,7 @@
       <c r="B8" s="56"/>
       <c r="C8" s="57"/>
       <c r="D8" s="58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="59"/>
       <c r="F8" s="54"/>
@@ -3694,7 +3694,7 @@
       <c r="B9" s="56"/>
       <c r="C9" s="60"/>
       <c r="D9" s="58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="59"/>
       <c r="F9" s="54"/>
@@ -3715,7 +3715,7 @@
       <c r="B10" s="56"/>
       <c r="C10" s="61"/>
       <c r="D10" s="58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="54"/>
       <c r="F10" s="54"/>
@@ -3765,7 +3765,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="119" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" s="119"/>
       <c r="H12" s="119"/>
@@ -3782,7 +3782,7 @@
     <row r="13" spans="1:17">
       <c r="A13" s="48"/>
       <c r="B13" s="121" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="119"/>
       <c r="D13" s="119"/>
@@ -3812,7 +3812,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="69" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F14" s="54"/>
       <c r="G14" s="54"/>
@@ -3866,7 +3866,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="69" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
@@ -3884,7 +3884,7 @@
     <row r="17" spans="1:17">
       <c r="A17" s="48"/>
       <c r="B17" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="29">
         <v>5</v>
@@ -3893,7 +3893,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="69" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
@@ -3911,14 +3911,14 @@
     <row r="18" spans="1:17">
       <c r="A18" s="48"/>
       <c r="B18" s="67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>38</v>
+        <v>245</v>
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
@@ -3936,15 +3936,15 @@
     <row r="19" spans="1:17">
       <c r="A19" s="48"/>
       <c r="B19" s="67" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C19" s="116" t="str">
         <f>IF(C18="Internal", "High","Low")</f>
-        <v>High</v>
+        <v>Low</v>
       </c>
       <c r="D19" s="68"/>
       <c r="E19" s="69" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F19" s="54"/>
       <c r="G19" s="54"/>
@@ -3962,14 +3962,14 @@
     <row r="20" spans="1:17">
       <c r="A20" s="48"/>
       <c r="B20" s="67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D20" s="68"/>
       <c r="E20" s="69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F20" s="54"/>
       <c r="G20" s="54"/>
@@ -3987,7 +3987,7 @@
     <row r="21" spans="1:17">
       <c r="A21" s="48"/>
       <c r="B21" s="67" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C21" s="31" t="str">
         <f>IF(C20="FPWM", "High","Low")</f>
@@ -3995,7 +3995,7 @@
       </c>
       <c r="D21" s="68"/>
       <c r="E21" s="69" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F21" s="54"/>
       <c r="G21" s="54"/>
@@ -4013,7 +4013,7 @@
     <row r="22" spans="1:17" ht="25.5">
       <c r="A22" s="48"/>
       <c r="B22" s="67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="32">
         <v>100000</v>
@@ -4022,7 +4022,7 @@
         <v>28</v>
       </c>
       <c r="E22" s="69" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F22" s="54"/>
       <c r="G22" s="54"/>
@@ -4040,7 +4040,7 @@
     <row r="23" spans="1:17">
       <c r="A23" s="48"/>
       <c r="B23" s="70" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C23" s="33">
         <f>R_5/(Vout/1.2-1)</f>
@@ -4050,7 +4050,7 @@
         <v>28</v>
       </c>
       <c r="E23" s="69" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F23" s="54"/>
       <c r="G23" s="54"/>
@@ -4068,7 +4068,7 @@
     <row r="24" spans="1:17">
       <c r="A24" s="48"/>
       <c r="B24" s="67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="29">
         <v>5</v>
@@ -4077,7 +4077,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="69" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" s="54"/>
       <c r="G24" s="54"/>
@@ -4095,17 +4095,17 @@
     <row r="25" spans="1:17">
       <c r="A25" s="48"/>
       <c r="B25" s="67" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="23">
         <f>50/Iout_limit</f>
         <v>10</v>
       </c>
       <c r="D25" s="68" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E25" s="69" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" s="54"/>
       <c r="G25" s="54"/>
@@ -4123,7 +4123,7 @@
     <row r="26" spans="1:17" ht="25.5">
       <c r="A26" s="48"/>
       <c r="B26" s="67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C26" s="34">
         <f>IF((Vout&gt;Vin_min), SQRT((Vout-Vin_min)/Vin_min)*Ioutmax, 1/SQRT(12)*Vout*(1-Vout/Vin_max)/L/fsw)</f>
@@ -4151,7 +4151,7 @@
     <row r="27" spans="1:17" ht="25.5">
       <c r="A27" s="48"/>
       <c r="B27" s="67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C27" s="34">
         <f>IF((Vin_max&gt;Vout), IF(Vin_max&lt;(2*Vout), Ioutmax*SQRT(Vout*(Vin_max-Vout)/Vin_max/Vin_max), Ioutmax/2), IF(Vin_min&gt;Vout/2, 1/SQRT(12)*Vin_min*(1-Vin_min/Vout)/L/fsw, 1/SQRT(12)*Vout/4/L/fsw))</f>
@@ -4234,7 +4234,7 @@
     <row r="30" spans="1:17">
       <c r="A30" s="48"/>
       <c r="B30" s="67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="35">
         <v>1000</v>
@@ -4243,7 +4243,7 @@
         <v>6</v>
       </c>
       <c r="E30" s="69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F30" s="54"/>
       <c r="G30" s="54"/>
@@ -4261,7 +4261,7 @@
     <row r="31" spans="1:17">
       <c r="A31" s="48"/>
       <c r="B31" s="70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="37">
         <f>1/2.8/C29/C30</f>
@@ -4272,7 +4272,7 @@
       </c>
       <c r="E31" s="69"/>
       <c r="F31" s="126" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G31" s="126"/>
       <c r="H31" s="126"/>
@@ -4289,7 +4289,7 @@
     <row r="32" spans="1:17" ht="25.5">
       <c r="A32" s="48"/>
       <c r="B32" s="67" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C32" s="38">
         <v>0.01</v>
@@ -4298,7 +4298,7 @@
         <v>20</v>
       </c>
       <c r="E32" s="69" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F32" s="97"/>
       <c r="G32" s="98"/>
@@ -4316,7 +4316,7 @@
     <row r="33" spans="1:17" ht="27" customHeight="1">
       <c r="A33" s="48"/>
       <c r="B33" s="70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="39">
         <f>MAX((Vout-Vin_min)/Vout/fsw*Ioutmax/dVoutpkpk, 1/8/fsw*(ILpeak_max-ILvalley_max)/dVoutpkpk)</f>
@@ -4344,7 +4344,7 @@
     <row r="34" spans="1:17">
       <c r="A34" s="48"/>
       <c r="B34" s="128" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C34" s="139">
         <v>2.8E-5</v>
@@ -4353,7 +4353,7 @@
         <v>9</v>
       </c>
       <c r="E34" s="134" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F34" s="154"/>
       <c r="G34" s="137"/>
@@ -4390,7 +4390,7 @@
     <row r="36" spans="1:17" ht="15.75" customHeight="1">
       <c r="A36" s="48"/>
       <c r="B36" s="128" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C36" s="139">
         <v>1E-3</v>
@@ -4399,7 +4399,7 @@
         <v>9</v>
       </c>
       <c r="E36" s="134" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F36" s="154"/>
       <c r="G36" s="137"/>
@@ -4436,7 +4436,7 @@
     <row r="38" spans="1:17">
       <c r="A38" s="48"/>
       <c r="B38" s="128" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C38" s="157">
         <v>8.0000000000000002E-3</v>
@@ -4445,7 +4445,7 @@
         <v>28</v>
       </c>
       <c r="E38" s="134" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F38" s="154"/>
       <c r="G38" s="137"/>
@@ -4482,7 +4482,7 @@
     <row r="40" spans="1:17">
       <c r="A40" s="48"/>
       <c r="B40" s="128" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C40" s="155">
         <v>0.05</v>
@@ -4491,7 +4491,7 @@
         <v>20</v>
       </c>
       <c r="E40" s="134" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F40" s="154"/>
       <c r="G40" s="137"/>
@@ -4528,7 +4528,7 @@
     <row r="42" spans="1:17">
       <c r="A42" s="48"/>
       <c r="B42" s="159" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="161">
         <f>Ioutmax*0.25/dVinpkpk/fsw</f>
@@ -4538,7 +4538,7 @@
         <v>9</v>
       </c>
       <c r="E42" s="134" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F42" s="154"/>
       <c r="G42" s="137"/>
@@ -4575,7 +4575,7 @@
     <row r="44" spans="1:17">
       <c r="A44" s="48"/>
       <c r="B44" s="128" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" s="139">
         <v>1E-4</v>
@@ -4621,14 +4621,14 @@
     <row r="46" spans="1:17">
       <c r="A46" s="48"/>
       <c r="B46" s="128" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C46" s="130">
         <v>0.94</v>
       </c>
       <c r="D46" s="132"/>
       <c r="E46" s="134" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F46" s="136"/>
       <c r="G46" s="137"/>
@@ -4672,7 +4672,7 @@
       </c>
       <c r="D48" s="132"/>
       <c r="E48" s="134" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F48" s="136"/>
       <c r="G48" s="137"/>
@@ -4709,7 +4709,7 @@
     <row r="50" spans="1:17" ht="25.5">
       <c r="A50" s="48"/>
       <c r="B50" s="67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C50" s="39">
         <f>IF(Vout&gt;Vin_min, Vin_min^2*eff*(Vout-Vin_min)/(K*Ioutmax*fsw*Vout^2), (1-Vout/Vin_max)*Vout/(K*Ioutmax*fsw))</f>
@@ -4719,7 +4719,7 @@
         <v>5</v>
       </c>
       <c r="E50" s="69" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F50" s="54"/>
       <c r="G50" s="54"/>
@@ -4762,7 +4762,7 @@
     <row r="52" spans="1:17">
       <c r="A52" s="48"/>
       <c r="B52" s="67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C52" s="34">
         <f>IF(Vout&gt;Vin_min, ((Ioutmax/(Vin_min/Vout)/eff)^2+1/12*(Vin_min/L*(1-Vin_min/Vout)/fsw)^2)^0.5, ((Ioutmax^2+1/12*(Vout/L*(1-Vout/Vin_max)/fsw)^2)^0.5))</f>
@@ -4790,7 +4790,7 @@
     <row r="53" spans="1:17" ht="25.5" customHeight="1">
       <c r="A53" s="48"/>
       <c r="B53" s="67" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C53" s="34">
         <f>IF(Vout&gt;Vin_min, (Ioutmax/(Vin_min/Vout)/eff+(1/2*Vin_min/L*(1-Vin_min/Vout)/fsw)), Ioutmax+1/2*(Vout*(1-Vout/Vin_max)/L/fsw))</f>
@@ -4800,7 +4800,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="69" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F53" s="54"/>
       <c r="G53" s="72"/>
@@ -4818,7 +4818,7 @@
     <row r="54" spans="1:17" ht="14.45" customHeight="1">
       <c r="A54" s="48"/>
       <c r="B54" s="67" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C54" s="34">
         <f>(ILpeak_max+ILvalley_max)/2</f>
@@ -4828,7 +4828,7 @@
         <v>4</v>
       </c>
       <c r="E54" s="69" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F54" s="54"/>
       <c r="G54" s="72"/>
@@ -4846,7 +4846,7 @@
     <row r="55" spans="1:17">
       <c r="A55" s="48"/>
       <c r="B55" s="67" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C55" s="34">
         <f>IF(Vout&gt;Vin_min, (Ioutmax/(Vin_min/Vout)/eff-(1/2*Vin_min/L*(1-Vin_min/Vout)/fsw)), Ioutmax-1/2*(Vout*(1-Vout/Vin_max)/L/fsw))</f>
@@ -4872,7 +4872,7 @@
     <row r="56" spans="1:17">
       <c r="A56" s="48"/>
       <c r="B56" s="67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C56" s="94">
         <v>8</v>
@@ -4881,7 +4881,7 @@
         <v>4</v>
       </c>
       <c r="E56" s="69" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F56" s="54"/>
       <c r="G56" s="72"/>
@@ -4899,16 +4899,16 @@
     <row r="57" spans="1:17">
       <c r="A57" s="48"/>
       <c r="B57" s="74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C57" s="41">
         <v>0</v>
       </c>
       <c r="D57" s="68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E57" s="69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F57" s="54"/>
       <c r="G57" s="72"/>
@@ -4926,17 +4926,17 @@
     <row r="58" spans="1:17">
       <c r="A58" s="48"/>
       <c r="B58" s="70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C58" s="42" t="str">
         <f>IF((C57=0), "floating", 3*R_7/C57)</f>
         <v>floating</v>
       </c>
       <c r="D58" s="68" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E58" s="69" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F58" s="54"/>
       <c r="G58" s="54"/>
@@ -4954,13 +4954,13 @@
     <row r="59" spans="1:17">
       <c r="A59" s="48"/>
       <c r="B59" s="125" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C59" s="123"/>
       <c r="D59" s="123"/>
       <c r="E59" s="123"/>
       <c r="F59" s="122" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G59" s="123"/>
       <c r="H59" s="123"/>
@@ -4986,7 +4986,7 @@
         <v>3</v>
       </c>
       <c r="E60" s="117" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F60" s="54"/>
       <c r="G60" s="54"/>
@@ -5030,7 +5030,7 @@
     <row r="62" spans="1:17" ht="12.75" customHeight="1">
       <c r="A62" s="75"/>
       <c r="B62" s="67" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C62" s="31" t="str">
         <f>IF((Vin_LP &gt; Vout_LP),"Buck","Boost")</f>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="D62" s="68"/>
       <c r="E62" s="69" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F62" s="54"/>
       <c r="G62" s="54"/>
@@ -5056,17 +5056,17 @@
     <row r="63" spans="1:17" ht="12.75" customHeight="1">
       <c r="A63" s="75"/>
       <c r="B63" s="67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C63" s="43">
         <f>17+Ioutmax/2.5</f>
         <v>19</v>
       </c>
       <c r="D63" s="68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E63" s="69" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F63" s="54"/>
       <c r="G63" s="54"/>
@@ -5084,7 +5084,7 @@
     <row r="64" spans="1:17" ht="12.75" customHeight="1">
       <c r="A64" s="75"/>
       <c r="B64" s="67" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C64" s="31">
         <f>IF((Op_mode="Buck"), Ioutmax/2/PI()/Vout_LP/(Cout_c+Cout_e), Ioutmax/PI()/Vout_LP/(Cout_c+Cout_e))</f>
@@ -5094,7 +5094,7 @@
         <v>6</v>
       </c>
       <c r="E64" s="69" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F64" s="54"/>
       <c r="G64" s="54"/>
@@ -5112,7 +5112,7 @@
     <row r="65" spans="1:17" ht="12.75" customHeight="1">
       <c r="A65" s="75"/>
       <c r="B65" s="67" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C65" s="31">
         <f>IF(Op_mode="Boost", Vout_LP*(eff*Vin_LP/Vout_LP)^2/2/PI()/L/Ioutmax, "No RPHZ")</f>
@@ -5122,7 +5122,7 @@
         <v>6</v>
       </c>
       <c r="E65" s="69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F65" s="54"/>
       <c r="G65" s="54"/>
@@ -5140,7 +5140,7 @@
     <row r="66" spans="1:17" ht="12.75" customHeight="1">
       <c r="A66" s="75"/>
       <c r="B66" s="67" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C66" s="31">
         <f>1/2/PI()/Cout_e/ESR</f>
@@ -5150,7 +5150,7 @@
         <v>6</v>
       </c>
       <c r="E66" s="69" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F66" s="54"/>
       <c r="G66" s="54"/>
@@ -5195,16 +5195,16 @@
     <row r="68" spans="1:17" ht="12.75" customHeight="1">
       <c r="A68" s="75"/>
       <c r="B68" s="67" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C68" s="76">
         <v>1.9000000000000001E-4</v>
       </c>
       <c r="D68" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="E68" s="69" t="s">
         <v>124</v>
-      </c>
-      <c r="E68" s="69" t="s">
-        <v>125</v>
       </c>
       <c r="F68" s="54"/>
       <c r="G68" s="54"/>
@@ -5222,7 +5222,7 @@
     <row r="69" spans="1:17">
       <c r="A69" s="75"/>
       <c r="B69" s="70" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C69" s="25">
         <f>IF(Op_mode="Boost", 2*PI()*fco*(Cout_c+Cout_e)*Vout/1.129/gm_PS/(eff*Vin_LP/Vout_LP)/gm_EA, 2*PI()*fco*(Cout_c+Cout_e)*Vout/1.129/gm_PS/gm_EA)</f>
@@ -5248,7 +5248,7 @@
     <row r="70" spans="1:17">
       <c r="A70" s="75"/>
       <c r="B70" s="67" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C70" s="22">
         <v>487000</v>
@@ -5257,7 +5257,7 @@
         <v>28</v>
       </c>
       <c r="E70" s="68" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F70" s="54"/>
       <c r="G70" s="54"/>
@@ -5275,7 +5275,7 @@
     <row r="71" spans="1:17">
       <c r="A71" s="75"/>
       <c r="B71" s="70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C71" s="39">
         <f>1/(2*PI()*(fco/10)*(Rcomp+2000))</f>
@@ -5285,7 +5285,7 @@
         <v>9</v>
       </c>
       <c r="E71" s="68" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F71" s="54"/>
       <c r="G71" s="54"/>
@@ -5303,7 +5303,7 @@
     <row r="72" spans="1:17">
       <c r="A72" s="75"/>
       <c r="B72" s="67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C72" s="40">
         <v>4.7000000000000003E-10</v>
@@ -5328,7 +5328,7 @@
     <row r="73" spans="1:17">
       <c r="A73" s="75"/>
       <c r="B73" s="67" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C73" s="25">
         <f>1/2/PI()/(Rcomp+2000)/Ccomp</f>
@@ -5338,7 +5338,7 @@
         <v>6</v>
       </c>
       <c r="E73" s="68" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F73" s="54"/>
       <c r="G73" s="54"/>
@@ -5356,7 +5356,7 @@
     <row r="74" spans="1:17" ht="38.25">
       <c r="A74" s="75"/>
       <c r="B74" s="70" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C74" s="44">
         <f>Ccomp*(IF(fzRHP&gt;fz_ESR, (Cout_e*ESR/Rcomp)/(Ccomp-Cout_e*ESR/Rcomp), (1/2/PI()/fzRHP/Rcomp)/(Ccomp-1/2/PI()/fzRHP/Rcomp)))</f>
@@ -5366,7 +5366,7 @@
         <v>9</v>
       </c>
       <c r="E74" s="69" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F74" s="71"/>
       <c r="G74" s="54"/>
@@ -5384,7 +5384,7 @@
     <row r="75" spans="1:17">
       <c r="A75" s="75"/>
       <c r="B75" s="77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C75" s="45">
         <v>1.7999999999999999E-11</v>
@@ -5409,7 +5409,7 @@
     <row r="76" spans="1:17">
       <c r="A76" s="75"/>
       <c r="B76" s="77" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C76" s="26">
         <f>1/2/PI()/(Rcomp+2000)/(Ccomp*(Cp+0.000000000003)/(Ccomp+Cp+0.000000000003))</f>
@@ -5419,7 +5419,7 @@
         <v>6</v>
       </c>
       <c r="E76" s="78" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F76" s="54"/>
       <c r="G76" s="54"/>
@@ -5437,7 +5437,7 @@
     <row r="77" spans="1:17">
       <c r="A77" s="75"/>
       <c r="B77" s="121" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C77" s="119"/>
       <c r="D77" s="119"/>
@@ -5467,7 +5467,7 @@
         <v>3</v>
       </c>
       <c r="E78" s="79" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F78" s="54"/>
       <c r="G78" s="54"/>
@@ -5495,7 +5495,7 @@
         <v>4</v>
       </c>
       <c r="E79" s="69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F79" s="54"/>
       <c r="G79" s="54"/>
@@ -5523,7 +5523,7 @@
         <v>4</v>
       </c>
       <c r="E80" s="69" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F80" s="54"/>
       <c r="G80" s="54"/>
@@ -5541,7 +5541,7 @@
     <row r="81" spans="1:17">
       <c r="A81" s="75"/>
       <c r="B81" s="67" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C81" s="46">
         <f>IF(Vin_eff&lt;Vout, (Ioutmax/(Vin_eff/Vout)/eff-(1/2*Vin_eff/L*(1-Vin_eff/Vout)/fsw)),Ioutmax-1/2*(Vout*(1-Vout/Vin_eff)/L/fsw))</f>
@@ -5551,7 +5551,7 @@
         <v>4</v>
       </c>
       <c r="E81" s="69" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F81" s="54"/>
       <c r="G81" s="54"/>
@@ -5596,7 +5596,7 @@
     <row r="83" spans="1:17" ht="25.5">
       <c r="A83" s="48"/>
       <c r="B83" s="67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C83" s="29">
         <v>1.8200000000000001E-2</v>
@@ -5605,7 +5605,7 @@
         <v>28</v>
       </c>
       <c r="E83" s="69" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F83" s="54"/>
       <c r="G83" s="72"/>
@@ -5623,16 +5623,16 @@
     <row r="84" spans="1:17" hidden="1">
       <c r="A84" s="48"/>
       <c r="B84" s="67" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C84" s="40">
         <v>5.0000000000000001E-9</v>
       </c>
       <c r="D84" s="68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E84" s="69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F84" s="54"/>
       <c r="G84" s="72"/>
@@ -5650,7 +5650,7 @@
     <row r="85" spans="1:17" hidden="1">
       <c r="A85" s="48"/>
       <c r="B85" s="67" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C85" s="40">
         <v>2.0000000000000001E-10</v>
@@ -5659,7 +5659,7 @@
         <v>9</v>
       </c>
       <c r="E85" s="69" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F85" s="54"/>
       <c r="G85" s="72"/>
@@ -5677,7 +5677,7 @@
     <row r="86" spans="1:17">
       <c r="A86" s="48"/>
       <c r="B86" s="67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C86" s="95">
         <v>1.3000000000000001E-8</v>
@@ -5686,7 +5686,7 @@
         <v>8</v>
       </c>
       <c r="E86" s="69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F86" s="54"/>
       <c r="G86" s="80"/>
@@ -5704,7 +5704,7 @@
     <row r="87" spans="1:17">
       <c r="A87" s="48"/>
       <c r="B87" s="67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C87" s="95">
         <v>1.3000000000000001E-8</v>
@@ -5713,7 +5713,7 @@
         <v>8</v>
       </c>
       <c r="E87" s="69" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F87" s="54"/>
       <c r="G87" s="54"/>
@@ -5731,7 +5731,7 @@
     <row r="88" spans="1:17" ht="25.5">
       <c r="A88" s="48"/>
       <c r="B88" s="67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C88" s="29">
         <v>2.86E-2</v>
@@ -5740,7 +5740,7 @@
         <v>28</v>
       </c>
       <c r="E88" s="69" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F88" s="54"/>
       <c r="G88" s="54"/>
@@ -5758,16 +5758,16 @@
     <row r="89" spans="1:17" hidden="1">
       <c r="A89" s="48"/>
       <c r="B89" s="67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C89" s="40">
         <v>5.0000000000000001E-9</v>
       </c>
       <c r="D89" s="68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E89" s="69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F89" s="54"/>
       <c r="G89" s="54"/>
@@ -5785,16 +5785,16 @@
     <row r="90" spans="1:17" hidden="1">
       <c r="A90" s="48"/>
       <c r="B90" s="67" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C90" s="40">
         <v>5.0000000000000001E-9</v>
       </c>
       <c r="D90" s="68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E90" s="69" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F90" s="54"/>
       <c r="G90" s="54"/>
@@ -5812,7 +5812,7 @@
     <row r="91" spans="1:17">
       <c r="A91" s="48"/>
       <c r="B91" s="67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C91" s="76">
         <v>1E-8</v>
@@ -5821,7 +5821,7 @@
         <v>8</v>
       </c>
       <c r="E91" s="69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F91" s="54"/>
       <c r="G91" s="54"/>
@@ -5839,7 +5839,7 @@
     <row r="92" spans="1:17">
       <c r="A92" s="48"/>
       <c r="B92" s="67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C92" s="23">
         <v>0.8</v>
@@ -5866,7 +5866,7 @@
     <row r="93" spans="1:17" ht="25.5">
       <c r="A93" s="48"/>
       <c r="B93" s="67" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C93" s="29">
         <v>1.43E-2</v>
@@ -5875,7 +5875,7 @@
         <v>28</v>
       </c>
       <c r="E93" s="69" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F93" s="54"/>
       <c r="G93" s="72"/>
@@ -5893,7 +5893,7 @@
     <row r="94" spans="1:17">
       <c r="A94" s="48"/>
       <c r="B94" s="67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C94" s="76">
         <v>8.9999999999999995E-9</v>
@@ -5902,7 +5902,7 @@
         <v>8</v>
       </c>
       <c r="E94" s="69" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F94" s="54"/>
       <c r="G94" s="80"/>
@@ -5920,7 +5920,7 @@
     <row r="95" spans="1:17">
       <c r="A95" s="48"/>
       <c r="B95" s="67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C95" s="76">
         <v>1.3000000000000001E-8</v>
@@ -5929,7 +5929,7 @@
         <v>8</v>
       </c>
       <c r="E95" s="69" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F95" s="54"/>
       <c r="G95" s="54"/>
@@ -5947,7 +5947,7 @@
     <row r="96" spans="1:17" ht="25.5">
       <c r="A96" s="48"/>
       <c r="B96" s="67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C96" s="29">
         <v>1.2999999999999999E-2</v>
@@ -5956,7 +5956,7 @@
         <v>28</v>
       </c>
       <c r="E96" s="69" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F96" s="54"/>
       <c r="G96" s="54"/>
@@ -5974,7 +5974,7 @@
     <row r="97" spans="1:17">
       <c r="A97" s="48"/>
       <c r="B97" s="67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C97" s="76">
         <v>2E-8</v>
@@ -5983,7 +5983,7 @@
         <v>8</v>
       </c>
       <c r="E97" s="69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F97" s="54"/>
       <c r="G97" s="54"/>
@@ -6001,7 +6001,7 @@
     <row r="98" spans="1:17">
       <c r="A98" s="48"/>
       <c r="B98" s="67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C98" s="33">
         <v>1</v>
@@ -6028,7 +6028,7 @@
     <row r="99" spans="1:17">
       <c r="A99" s="48"/>
       <c r="B99" s="67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C99" s="47">
         <v>0</v>
@@ -6037,7 +6037,7 @@
         <v>9</v>
       </c>
       <c r="E99" s="69" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F99" s="54"/>
       <c r="G99" s="54"/>
@@ -6055,7 +6055,7 @@
     <row r="100" spans="1:17">
       <c r="A100" s="48"/>
       <c r="B100" s="67" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C100" s="47">
         <v>0</v>
@@ -6064,7 +6064,7 @@
         <v>9</v>
       </c>
       <c r="E100" s="69" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F100" s="54"/>
       <c r="G100" s="54"/>
@@ -6082,16 +6082,16 @@
     <row r="101" spans="1:17">
       <c r="A101" s="48"/>
       <c r="B101" s="74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C101" s="23">
         <v>2</v>
       </c>
       <c r="D101" s="68" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E101" s="69" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F101" s="54"/>
       <c r="G101" s="54"/>
@@ -6109,7 +6109,7 @@
     <row r="102" spans="1:17">
       <c r="A102" s="48"/>
       <c r="B102" s="74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C102" s="25">
         <f>Rpcb*(ILrms^2)</f>
@@ -6119,7 +6119,7 @@
         <v>10</v>
       </c>
       <c r="E102" s="69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F102" s="54"/>
       <c r="G102" s="54"/>
@@ -6137,7 +6137,7 @@
     <row r="103" spans="1:17">
       <c r="A103" s="75"/>
       <c r="B103" s="67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C103" s="25">
         <f>(ILrms)^2*DCR*1000</f>
@@ -6165,7 +6165,7 @@
     <row r="104" spans="1:17" ht="37.9" customHeight="1">
       <c r="A104" s="75"/>
       <c r="B104" s="67" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C104" s="22">
         <v>50</v>
@@ -6174,7 +6174,7 @@
         <v>10</v>
       </c>
       <c r="E104" s="69" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F104" s="54"/>
       <c r="G104" s="54"/>
@@ -6192,7 +6192,7 @@
     <row r="105" spans="1:17">
       <c r="A105" s="75"/>
       <c r="B105" s="74" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C105" s="25">
         <f>IF(Vin_eff&lt;Vout, ((0.001+0.00000001*fsw)*IF(AND(Vout&gt;Vin_eff, Vin_eff&gt;6.2), Vin_eff, Vout)+(1-Vin_eff/Vout)*ILrms^2*BST_LS_Rdson+(Vin_eff/Vout)*ILrms^2*BST_HS_Rdson+1/2*ILpeak*(Vout+BST_HS_Vd)*BST_LS_rise_time*fsw+1/2*ILvalley*(Vout+BST_HS_Vd)*BST_LS_fall_time*fsw+1/2*0.0000000005*(Vout+BST_HS_Vd)*(Vout+BST_HS_Vd)*fsw+(ILpeak+ILvalley)*BST_HS_Vd*BST_HS_dead_time*fsw+Vout*0.000000005*fsw)*1000+ (ILrms)^2*(BUCK_HS_Rdson)*1000, ((0.001+(BUCK_HS_Qg+BUCK_LS_Qg)*fsw)*IF(AND(Vin_eff&gt;Vout, Vout&gt;6.2), Vout, Vin_eff)+BST_HS_Rdson*ILrms^2)*1000+ ((Vout/Vin_eff)*ILrms^2*BUCK_HS_Rdson+1/2*ILpeak*(Vin_eff+BUCK_LS_Vd)*BUCK_HS_fall_time*fsw+1/2*ILvalley*(Vin_eff+BUCK_LS_Vd)*BUCK_HS_rise_time*fsw+1/2*BUCK_HS_Coss*(Vin_eff+BUCK_LS_Vd)*(Vin_eff+BUCK_LS_Vd)*fsw)*1000+ ((1-Vout/Vin_eff)*ILrms^2*BUCK_LS_Rdson+(ILpeak+ILvalley)*BUCK_LS_Vd*BUCK_LS_dead_time*fsw+Vin_eff*BUCK_LS_Qrr*fsw)*1000)</f>
@@ -6202,7 +6202,7 @@
         <v>10</v>
       </c>
       <c r="E105" s="69" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F105" s="54"/>
       <c r="G105" s="54"/>
@@ -6220,7 +6220,7 @@
     <row r="106" spans="1:17">
       <c r="A106" s="75"/>
       <c r="B106" s="81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C106" s="26">
         <f>Ioutmax*Ioutmax*R_1</f>
@@ -6230,7 +6230,7 @@
         <v>10</v>
       </c>
       <c r="E106" s="82" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F106" s="54"/>
       <c r="G106" s="54"/>
@@ -6248,7 +6248,7 @@
     <row r="107" spans="1:17">
       <c r="A107" s="75"/>
       <c r="B107" s="81" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C107" s="26">
         <f>IF(Vin_eff&lt;Vout, 2/3*C_bst_snubber*(Vout+BST_HS_Vd)*(Vout+BST_HS_Vd)*fsw*1000, 2/3*C_buck_snubber*(Vin_eff+BUCK_LS_Vd)*(Vin_eff+BUCK_LS_Vd)*fsw*1000)</f>
@@ -6258,7 +6258,7 @@
         <v>10</v>
       </c>
       <c r="E107" s="82" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F107" s="54"/>
       <c r="G107" s="54"/>
@@ -6276,7 +6276,7 @@
     <row r="108" spans="1:17">
       <c r="A108" s="75"/>
       <c r="B108" s="81" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C108" s="26">
         <f>IF(Vin_eff&lt;Vout, 1000*ESR*(G108+H108), 0)</f>
@@ -6286,7 +6286,7 @@
         <v>10</v>
       </c>
       <c r="E108" s="82" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F108" s="96">
         <f>ESR*Cout_c*Cout_e/(Cout_c+Cout_e)</f>
@@ -6313,7 +6313,7 @@
     <row r="109" spans="1:17">
       <c r="A109" s="75"/>
       <c r="B109" s="77" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C109" s="27">
         <f>IF(Vin_eff&lt;Vout, Vout*Ioutmax/(Vout*Ioutmax+(C102+C103+C104+C105+C106+C107+C108)/1000), Vout*Ioutmax/(Vout*Ioutmax+(C102+C103+C104+C105+C106+C107)/1000))</f>
@@ -6321,7 +6321,7 @@
       </c>
       <c r="D109" s="78"/>
       <c r="E109" s="82" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F109" s="54"/>
       <c r="G109" s="54"/>
@@ -6339,16 +6339,16 @@
     <row r="110" spans="1:17" ht="25.5">
       <c r="A110" s="75"/>
       <c r="B110" s="67" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C110" s="22">
         <v>33</v>
       </c>
       <c r="D110" s="68" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E110" s="69" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F110" s="54"/>
       <c r="G110" s="54"/>
@@ -6366,17 +6366,17 @@
     <row r="111" spans="1:17" ht="26.25" thickBot="1">
       <c r="A111" s="75"/>
       <c r="B111" s="83" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C111" s="28">
         <f>C110*(C105)/1000</f>
         <v>70.569539999417671</v>
       </c>
       <c r="D111" s="84" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E111" s="85" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F111" s="86"/>
       <c r="G111" s="86"/>
@@ -6745,7 +6745,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="63.75">
       <c r="A1" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -6753,7 +6753,7 @@
     </row>
     <row r="3" spans="1:1" ht="76.5">
       <c r="A3" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -6761,7 +6761,7 @@
     </row>
     <row r="5" spans="1:1" ht="51">
       <c r="A5" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -6769,7 +6769,7 @@
     </row>
     <row r="7" spans="1:1" ht="76.5">
       <c r="A7" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -6777,7 +6777,7 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -6827,11 +6827,11 @@
   <sheetData>
     <row r="1" spans="1:34" ht="14.25" thickTop="1" thickBot="1">
       <c r="A1" s="165" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="167"/>
       <c r="C1" s="165" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" s="166"/>
       <c r="E1" s="166"/>
@@ -6841,7 +6841,7 @@
       <c r="I1" s="166"/>
       <c r="J1" s="167"/>
       <c r="K1" s="165" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L1" s="166"/>
       <c r="M1" s="166"/>
@@ -6849,11 +6849,11 @@
       <c r="O1" s="166"/>
       <c r="P1" s="166"/>
       <c r="Q1" s="165" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R1" s="167"/>
       <c r="S1" s="165" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T1" s="166"/>
       <c r="U1" s="166"/>
@@ -6861,11 +6861,11 @@
       <c r="W1" s="166"/>
       <c r="X1" s="167"/>
       <c r="Y1" s="165" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z1" s="167"/>
       <c r="AA1" s="166" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB1" s="166"/>
       <c r="AC1" s="166"/>
@@ -6874,100 +6874,100 @@
     <row r="2" spans="1:34" ht="26.25" thickTop="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="Y2" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>138</v>
-      </c>
       <c r="AF2" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AG2" s="21" t="s">
         <v>24</v>
       </c>
       <c r="AH2" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -7090,13 +7090,13 @@
         <v>77.912448207661441</v>
       </c>
       <c r="AF3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AG3">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="AH3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -7219,13 +7219,13 @@
         <v>69.885933337357542</v>
       </c>
       <c r="AF4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AG4">
         <v>100000</v>
       </c>
       <c r="AH4" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -7348,7 +7348,7 @@
         <v>62.960319852833209</v>
       </c>
       <c r="AF5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AG5">
         <v>6.2599999999999996E-11</v>
@@ -7477,7 +7477,7 @@
         <v>57.462918935811544</v>
       </c>
       <c r="AF6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AG6">
         <f>0.1*MIN(Vin, Vout)</f>

</xml_diff>